<commit_message>
Card __innit__ change to excel initialization
</commit_message>
<xml_diff>
--- a/cards_data.xlsx
+++ b/cards_data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ddnikulin/Documents/GitHub/RL_in_Hearstone_Battlegrounds/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0A5F29FA-E09E-6E49-9A98-DD44BCD2EA0E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{44C332C6-222C-894F-85B6-8A846C9699AB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="5800" yWindow="-18820" windowWidth="28240" windowHeight="17240" xr2:uid="{9245884C-8768-584D-B284-F4567C4CADCB}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="15">
   <si>
     <t>card_name</t>
   </si>
@@ -73,9 +73,6 @@
     <t>PlayedCardBuffMechanic</t>
   </si>
   <si>
-    <t>test</t>
-  </si>
-  <si>
     <t>Tavern_Tipper</t>
   </si>
   <si>
@@ -83,9 +80,6 @@
   </si>
   <si>
     <t>Demon</t>
-  </si>
-  <si>
-    <t>PlayedCardBuffMechanic,pivo</t>
   </si>
 </sst>
 </file>
@@ -438,10 +432,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F2E0D5F8-3BEF-E143-9FC9-23807AC53446}">
-  <dimension ref="A1:H5"/>
+  <dimension ref="A1:H4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H3" sqref="H3"/>
+      <selection activeCell="A3" sqref="A3:XFD3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -513,10 +507,10 @@
         <v>12</v>
       </c>
       <c r="B3">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C3">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D3" t="s">
         <v>9</v>
@@ -529,9 +523,6 @@
       </c>
       <c r="G3">
         <v>17</v>
-      </c>
-      <c r="H3" t="s">
-        <v>16</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.2">
@@ -539,44 +530,21 @@
         <v>13</v>
       </c>
       <c r="B4">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="C4">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="D4" t="s">
         <v>9</v>
       </c>
       <c r="E4" t="s">
-        <v>10</v>
+        <v>14</v>
       </c>
       <c r="F4">
         <v>1</v>
       </c>
       <c r="G4">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A5" t="s">
-        <v>14</v>
-      </c>
-      <c r="B5">
-        <v>4</v>
-      </c>
-      <c r="C5">
-        <v>4</v>
-      </c>
-      <c r="D5" t="s">
-        <v>9</v>
-      </c>
-      <c r="E5" t="s">
-        <v>15</v>
-      </c>
-      <c r="F5">
-        <v>1</v>
-      </c>
-      <c r="G5">
         <v>17</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Added Blazing_Skyfin to Card
</commit_message>
<xml_diff>
--- a/cards_data.xlsx
+++ b/cards_data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ddnikulin/Documents/GitHub/RL_in_Hearstone_Battlegrounds/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F02B19AC-076A-1A48-85EA-C043E4DDD19E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E4C3AA51-D70C-9548-AD3A-1DB913A0B203}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="5800" yWindow="-18820" windowWidth="28240" windowHeight="17240" xr2:uid="{9245884C-8768-584D-B284-F4567C4CADCB}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="23">
   <si>
     <t>card_name</t>
   </si>
@@ -459,7 +459,7 @@
   <dimension ref="A1:I8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H7" sqref="H7"/>
+      <selection activeCell="F13" sqref="F13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -639,7 +639,7 @@
         <v>11</v>
       </c>
       <c r="I6">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.2">
@@ -693,8 +693,11 @@
       <c r="G8">
         <v>17</v>
       </c>
+      <c r="H8" t="s">
+        <v>11</v>
+      </c>
       <c r="I8">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added tavern.eat_minion() and demons that eat
</commit_message>
<xml_diff>
--- a/cards_data.xlsx
+++ b/cards_data.xlsx
@@ -8,14 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ddnikulin/Documents/GitHub/RL_in_Hearstone_Battlegrounds/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{85BD6EE0-FE35-F044-A44E-316A7069C47A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9ABB819B-9183-BD48-8FCB-0606CA07902C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6560" yWindow="-17800" windowWidth="28240" windowHeight="17240" xr2:uid="{9245884C-8768-584D-B284-F4567C4CADCB}"/>
+    <workbookView xWindow="4180" yWindow="3320" windowWidth="28240" windowHeight="17240" xr2:uid="{9245884C-8768-584D-B284-F4567C4CADCB}"/>
   </bookViews>
   <sheets>
     <sheet name="Лист1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="27">
   <si>
     <t>card_name</t>
   </si>
@@ -110,6 +110,12 @@
   </si>
   <si>
     <t>Saltscale_Honcho</t>
+  </si>
+  <si>
+    <t>Picky_Eater</t>
+  </si>
+  <si>
+    <t>Mind_Muck</t>
   </si>
 </sst>
 </file>
@@ -462,10 +468,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F2E0D5F8-3BEF-E143-9FC9-23807AC53446}">
-  <dimension ref="A1:I10"/>
+  <dimension ref="A1:I12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A10" sqref="A10"/>
+      <selection activeCell="A5" sqref="A5:XFD5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -590,59 +596,59 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:9" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>17</v>
+        <v>26</v>
       </c>
       <c r="B5">
         <v>3</v>
       </c>
       <c r="C5">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D5" t="s">
         <v>9</v>
       </c>
       <c r="E5" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="F5">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G5">
         <v>17</v>
       </c>
       <c r="H5" t="s">
-        <v>11</v>
+        <v>22</v>
       </c>
       <c r="I5">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="B6">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C6">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D6" t="s">
         <v>9</v>
       </c>
       <c r="E6" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="F6">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G6">
         <v>17</v>
       </c>
       <c r="H6" t="s">
-        <v>11</v>
+        <v>22</v>
       </c>
       <c r="I6">
         <v>0</v>
@@ -650,19 +656,19 @@
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B7">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="C7">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="D7" t="s">
         <v>9</v>
       </c>
       <c r="E7" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="F7">
         <v>1</v>
@@ -679,28 +685,28 @@
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="B8">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C8">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D8" t="s">
         <v>9</v>
       </c>
       <c r="E8" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="F8">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G8">
         <v>17</v>
       </c>
       <c r="H8" t="s">
-        <v>22</v>
+        <v>11</v>
       </c>
       <c r="I8">
         <v>0</v>
@@ -708,13 +714,13 @@
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="B9">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C9">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="D9" t="s">
         <v>9</v>
@@ -723,7 +729,7 @@
         <v>18</v>
       </c>
       <c r="F9">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G9">
         <v>17</v>
@@ -737,13 +743,13 @@
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="B10">
+        <v>2</v>
+      </c>
+      <c r="C10">
         <v>3</v>
-      </c>
-      <c r="C10">
-        <v>2</v>
       </c>
       <c r="D10" t="s">
         <v>9</v>
@@ -758,10 +764,68 @@
         <v>17</v>
       </c>
       <c r="H10" t="s">
+        <v>22</v>
+      </c>
+      <c r="I10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>19</v>
+      </c>
+      <c r="B11">
+        <v>2</v>
+      </c>
+      <c r="C11">
+        <v>4</v>
+      </c>
+      <c r="D11" t="s">
+        <v>9</v>
+      </c>
+      <c r="E11" t="s">
+        <v>18</v>
+      </c>
+      <c r="F11">
+        <v>2</v>
+      </c>
+      <c r="G11">
+        <v>17</v>
+      </c>
+      <c r="H11" t="s">
         <v>11</v>
       </c>
-      <c r="I10">
-        <v>1</v>
+      <c r="I11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>24</v>
+      </c>
+      <c r="B12">
+        <v>3</v>
+      </c>
+      <c r="C12">
+        <v>2</v>
+      </c>
+      <c r="D12" t="s">
+        <v>9</v>
+      </c>
+      <c r="E12" t="s">
+        <v>18</v>
+      </c>
+      <c r="F12">
+        <v>1</v>
+      </c>
+      <c r="G12">
+        <v>17</v>
+      </c>
+      <c r="H12" t="s">
+        <v>11</v>
+      </c>
+      <c r="I12">
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added trigger() method instead of tigger_buffs() method
</commit_message>
<xml_diff>
--- a/cards_data.xlsx
+++ b/cards_data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ddnikulin/Documents/GitHub/RL_in_Hearstone_Battlegrounds/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9ABB819B-9183-BD48-8FCB-0606CA07902C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A543D18C-500F-BB49-B567-0E55EB480B5A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4180" yWindow="3320" windowWidth="28240" windowHeight="17240" xr2:uid="{9245884C-8768-584D-B284-F4567C4CADCB}"/>
+    <workbookView xWindow="5160" yWindow="-18480" windowWidth="28240" windowHeight="17240" xr2:uid="{9245884C-8768-584D-B284-F4567C4CADCB}"/>
   </bookViews>
   <sheets>
     <sheet name="Лист1" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="28">
   <si>
     <t>card_name</t>
   </si>
@@ -116,13 +116,16 @@
   </si>
   <si>
     <t>Mind_Muck</t>
+  </si>
+  <si>
+    <t>Sellemental</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -130,6 +133,12 @@
       <family val="2"/>
       <charset val="204"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="14"/>
+      <color rgb="FF111827"/>
+      <name val="Menlo"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -152,13 +161,25 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="1">
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -468,10 +489,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F2E0D5F8-3BEF-E143-9FC9-23807AC53446}">
-  <dimension ref="A1:I12"/>
+  <dimension ref="A1:J14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5:XFD5"/>
+      <selection activeCell="K8" sqref="K8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -486,7 +507,7 @@
     <col min="8" max="8" width="26.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:10" ht="18" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -514,8 +535,9 @@
       <c r="I1" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J1" s="1"/>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>8</v>
       </c>
@@ -541,10 +563,10 @@
         <v>11</v>
       </c>
       <c r="I2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>12</v>
       </c>
@@ -567,10 +589,10 @@
         <v>17</v>
       </c>
       <c r="I3">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>13</v>
       </c>
@@ -592,11 +614,14 @@
       <c r="G4">
         <v>17</v>
       </c>
+      <c r="H4" t="s">
+        <v>22</v>
+      </c>
       <c r="I4">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>26</v>
       </c>
@@ -625,7 +650,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:9" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:10" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>25</v>
       </c>
@@ -654,7 +679,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>17</v>
       </c>
@@ -683,7 +708,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:10" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>23</v>
       </c>
@@ -712,44 +737,41 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:10" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>16</v>
+        <v>27</v>
       </c>
       <c r="B9">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="C9">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="D9" t="s">
         <v>9</v>
       </c>
       <c r="E9" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="F9">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G9">
         <v>17</v>
-      </c>
-      <c r="H9" t="s">
-        <v>11</v>
       </c>
       <c r="I9">
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="B10">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C10">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="D10" t="s">
         <v>9</v>
@@ -764,21 +786,21 @@
         <v>17</v>
       </c>
       <c r="H10" t="s">
-        <v>22</v>
+        <v>11</v>
       </c>
       <c r="I10">
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="B11">
         <v>2</v>
       </c>
       <c r="C11">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D11" t="s">
         <v>9</v>
@@ -787,27 +809,27 @@
         <v>18</v>
       </c>
       <c r="F11">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G11">
         <v>17</v>
       </c>
       <c r="H11" t="s">
-        <v>11</v>
+        <v>22</v>
       </c>
       <c r="I11">
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>24</v>
+        <v>19</v>
       </c>
       <c r="B12">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C12">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="D12" t="s">
         <v>9</v>
@@ -816,7 +838,7 @@
         <v>18</v>
       </c>
       <c r="F12">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G12">
         <v>17</v>
@@ -828,7 +850,40 @@
         <v>0</v>
       </c>
     </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
+        <v>24</v>
+      </c>
+      <c r="B13">
+        <v>3</v>
+      </c>
+      <c r="C13">
+        <v>2</v>
+      </c>
+      <c r="D13" t="s">
+        <v>9</v>
+      </c>
+      <c r="E13" t="s">
+        <v>18</v>
+      </c>
+      <c r="F13">
+        <v>1</v>
+      </c>
+      <c r="G13">
+        <v>17</v>
+      </c>
+      <c r="H13" t="s">
+        <v>11</v>
+      </c>
+      <c r="I13">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" ht="17" customHeight="1" x14ac:dyDescent="0.2"/>
   </sheetData>
+  <conditionalFormatting sqref="A1:A1048576">
+    <cfRule type="duplicateValues" dxfId="0" priority="1"/>
+  </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Fixed battlecry_mechanic and rerolls
Fixed battlecry_mechanic and rerolls
</commit_message>
<xml_diff>
--- a/cards_data.xlsx
+++ b/cards_data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ddnikulin/Documents/GitHub/RL_in_Hearstone_Battlegrounds/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6D8822B5-03BD-F04E-A38B-F04298CB9CF1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DFB423C6-DABC-204D-B962-3AD3E15E621B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="3780" yWindow="3560" windowWidth="28240" windowHeight="17240" xr2:uid="{9245884C-8768-584D-B284-F4567C4CADCB}"/>
   </bookViews>
@@ -504,7 +504,7 @@
   <dimension ref="A1:L15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K13" sqref="K13"/>
+      <selection activeCell="K6" sqref="K6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -646,7 +646,7 @@
         <v>1</v>
       </c>
       <c r="K4">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="5" spans="1:12" ht="17" customHeight="1" x14ac:dyDescent="0.2">
@@ -678,7 +678,7 @@
         <v>1</v>
       </c>
       <c r="K5">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="6" spans="1:12" ht="17" customHeight="1" x14ac:dyDescent="0.2">
@@ -899,7 +899,7 @@
         <v>1</v>
       </c>
       <c r="K12">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.2">
@@ -931,7 +931,7 @@
         <v>1</v>
       </c>
       <c r="K13">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
Fixed sell battlecrymechanics problem
</commit_message>
<xml_diff>
--- a/cards_data.xlsx
+++ b/cards_data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ddnikulin/Documents/GitHub/RL_in_Hearstone_Battlegrounds/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DFB423C6-DABC-204D-B962-3AD3E15E621B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EA6E3D4A-639D-334B-8705-B241A414A313}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3780" yWindow="3560" windowWidth="28240" windowHeight="17240" xr2:uid="{9245884C-8768-584D-B284-F4567C4CADCB}"/>
+    <workbookView xWindow="5260" yWindow="-15440" windowWidth="28240" windowHeight="17240" xr2:uid="{9245884C-8768-584D-B284-F4567C4CADCB}"/>
   </bookViews>
   <sheets>
     <sheet name="Лист1" sheetId="1" r:id="rId1"/>
@@ -646,7 +646,7 @@
         <v>1</v>
       </c>
       <c r="K4">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="5" spans="1:12" ht="17" customHeight="1" x14ac:dyDescent="0.2">

</xml_diff>